<commit_message>
updated scripts, need to fix last 2
</commit_message>
<xml_diff>
--- a/40PA.xlsx
+++ b/40PA.xlsx
@@ -693,629 +693,629 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>17350</v>
+        <v>19251</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rafael Devers</t>
+          <t>Pete Alonso</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>NYM</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>614</v>
+        <v>685</v>
       </c>
       <c r="E5" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G5" t="n">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="H5" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" t="n">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="J5" t="n">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="K5" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="L5" t="n">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="M5" t="n">
-        <v>0.879</v>
+        <v>0.869</v>
       </c>
       <c r="N5" t="n">
-        <v>0.361</v>
+        <v>0.354</v>
       </c>
       <c r="O5" t="n">
-        <v>11.5</v>
+        <v>12.3</v>
       </c>
       <c r="P5" t="n">
-        <v>26.8</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="n">
-        <v>113.7</v>
+        <v>116.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>11579</v>
+        <v>17350</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bryce Harper</t>
+          <t>Rafael Devers</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>426</v>
+        <v>614</v>
       </c>
       <c r="E6" t="n">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H6" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="I6" t="n">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="J6" t="n">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="K6" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="L6" t="n">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="M6" t="n">
-        <v>0.877</v>
+        <v>0.879</v>
       </c>
       <c r="N6" t="n">
-        <v>0.38</v>
+        <v>0.361</v>
       </c>
       <c r="O6" t="n">
-        <v>12.8</v>
+        <v>11.5</v>
       </c>
       <c r="P6" t="n">
-        <v>18.1</v>
+        <v>26.8</v>
       </c>
       <c r="Q6" t="n">
-        <v>114.3</v>
+        <v>113.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>19251</v>
+        <v>18345</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Pete Alonso</t>
+          <t>Kyle Tucker</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>NYM</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>685</v>
+        <v>609</v>
       </c>
       <c r="E7" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="G7" t="n">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H7" t="n">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="I7" t="n">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="J7" t="n">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="K7" t="n">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="L7" t="n">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="M7" t="n">
-        <v>0.869</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="N7" t="n">
-        <v>0.354</v>
+        <v>0.353</v>
       </c>
       <c r="O7" t="n">
-        <v>12.3</v>
+        <v>10.1</v>
       </c>
       <c r="P7" t="n">
-        <v>32</v>
+        <v>23.9</v>
       </c>
       <c r="Q7" t="n">
-        <v>116.5</v>
+        <v>111.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>16535</v>
+        <v>14162</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Danny Jansen</t>
+          <t>Carlos Correa</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>248</v>
+        <v>590</v>
       </c>
       <c r="E8" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="H8" t="n">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="I8" t="n">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="J8" t="n">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="K8" t="n">
         <v>140</v>
       </c>
       <c r="L8" t="n">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="M8" t="n">
-        <v>0.855</v>
+        <v>0.834</v>
       </c>
       <c r="N8" t="n">
-        <v>0.368</v>
+        <v>0.363</v>
       </c>
       <c r="O8" t="n">
-        <v>13.1</v>
+        <v>11.4</v>
       </c>
       <c r="P8" t="n">
-        <v>12</v>
+        <v>20.7</v>
       </c>
       <c r="Q8" t="n">
-        <v>109.3</v>
+        <v>114.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>14162</v>
+        <v>19611</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Carlos Correa</t>
+          <t>Vladimir Guerrero Jr.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>590</v>
+        <v>706</v>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G9" t="n">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="H9" t="n">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="I9" t="n">
-        <v>130</v>
+        <v>103</v>
       </c>
       <c r="J9" t="n">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="K9" t="n">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="L9" t="n">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="M9" t="n">
-        <v>0.834</v>
+        <v>0.8179999999999999</v>
       </c>
       <c r="N9" t="n">
-        <v>0.363</v>
+        <v>0.348</v>
       </c>
       <c r="O9" t="n">
-        <v>11.4</v>
+        <v>11.2</v>
       </c>
       <c r="P9" t="n">
-        <v>20.7</v>
+        <v>19.3</v>
       </c>
       <c r="Q9" t="n">
-        <v>114.6</v>
+        <v>118.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>11609</v>
+        <v>11579</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Willson Contreras</t>
+          <t>Bryce Harper</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CHC</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>487</v>
+        <v>426</v>
       </c>
       <c r="E10" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F10" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G10" t="n">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="H10" t="n">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I10" t="n">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="J10" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="K10" t="n">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="L10" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M10" t="n">
-        <v>0.8149999999999999</v>
+        <v>0.877</v>
       </c>
       <c r="N10" t="n">
-        <v>0.364</v>
+        <v>0.38</v>
       </c>
       <c r="O10" t="n">
-        <v>10.5</v>
+        <v>12.8</v>
       </c>
       <c r="P10" t="n">
-        <v>15.2</v>
+        <v>18.1</v>
       </c>
       <c r="Q10" t="n">
-        <v>116.2</v>
+        <v>114.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>3473</v>
+        <v>13419</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Anthony Rizzo</t>
+          <t>Christian Walker</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>NYY</t>
+          <t>ARI</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>548</v>
+        <v>667</v>
       </c>
       <c r="E11" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F11" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H11" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I11" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="J11" t="n">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="K11" t="n">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="L11" t="n">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="M11" t="n">
-        <v>0.8169999999999999</v>
+        <v>0.804</v>
       </c>
       <c r="N11" t="n">
-        <v>0.349</v>
+        <v>0.359</v>
       </c>
       <c r="O11" t="n">
-        <v>10.9</v>
+        <v>11.5</v>
       </c>
       <c r="P11" t="n">
-        <v>16.4</v>
+        <v>16.9</v>
       </c>
       <c r="Q11" t="n">
-        <v>113.3</v>
+        <v>112.6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>19611</v>
+        <v>3473</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Vladimir Guerrero Jr.</t>
+          <t>Anthony Rizzo</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>NYY</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>706</v>
+        <v>548</v>
       </c>
       <c r="E12" t="n">
         <v>32</v>
       </c>
       <c r="F12" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G12" t="n">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="H12" t="n">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="I12" t="n">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="J12" t="n">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="K12" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L12" t="n">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="M12" t="n">
-        <v>0.8179999999999999</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="N12" t="n">
-        <v>0.348</v>
+        <v>0.349</v>
       </c>
       <c r="O12" t="n">
-        <v>11.2</v>
+        <v>10.9</v>
       </c>
       <c r="P12" t="n">
-        <v>19.3</v>
+        <v>16.4</v>
       </c>
       <c r="Q12" t="n">
-        <v>118.4</v>
+        <v>113.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>19197</v>
+        <v>11609</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Will Smith</t>
+          <t>Willson Contreras</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>LAD</t>
+          <t>CHC</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>578</v>
+        <v>487</v>
       </c>
       <c r="E13" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G13" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H13" t="n">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="I13" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="J13" t="n">
+        <v>144</v>
+      </c>
+      <c r="K13" t="n">
         <v>132</v>
       </c>
-      <c r="K13" t="n">
-        <v>127</v>
-      </c>
       <c r="L13" t="n">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="M13" t="n">
-        <v>0.8070000000000001</v>
+        <v>0.8149999999999999</v>
       </c>
       <c r="N13" t="n">
-        <v>0.352</v>
+        <v>0.364</v>
       </c>
       <c r="O13" t="n">
-        <v>10.3</v>
+        <v>10.5</v>
       </c>
       <c r="P13" t="n">
-        <v>14.9</v>
+        <v>15.2</v>
       </c>
       <c r="Q13" t="n">
-        <v>109</v>
+        <v>116.2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>18345</v>
+        <v>19197</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kyle Tucker</t>
+          <t>Will Smith</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>LAD</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>609</v>
+        <v>578</v>
       </c>
       <c r="E14" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F14" t="n">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H14" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="I14" t="n">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J14" t="n">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="K14" t="n">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L14" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M14" t="n">
-        <v>0.8080000000000001</v>
+        <v>0.8070000000000001</v>
       </c>
       <c r="N14" t="n">
-        <v>0.353</v>
+        <v>0.352</v>
       </c>
       <c r="O14" t="n">
-        <v>10.1</v>
+        <v>10.3</v>
       </c>
       <c r="P14" t="n">
-        <v>23.9</v>
+        <v>14.9</v>
       </c>
       <c r="Q14" t="n">
-        <v>111.3</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13419</v>
+        <v>16535</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Christian Walker</t>
+          <t>Danny Jansen</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>ARI</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>667</v>
+        <v>248</v>
       </c>
       <c r="E15" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="F15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H15" t="n">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I15" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="J15" t="n">
-        <v>152</v>
+        <v>171</v>
       </c>
       <c r="K15" t="n">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="L15" t="n">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="M15" t="n">
-        <v>0.804</v>
+        <v>0.855</v>
       </c>
       <c r="N15" t="n">
-        <v>0.359</v>
+        <v>0.368</v>
       </c>
       <c r="O15" t="n">
-        <v>11.5</v>
+        <v>13.1</v>
       </c>
       <c r="P15" t="n">
-        <v>16.9</v>
+        <v>12</v>
       </c>
       <c r="Q15" t="n">
-        <v>112.6</v>
+        <v>109.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>